<commit_message>
Adding dynamic List view
</commit_message>
<xml_diff>
--- a/untitled/Categories.xlsx
+++ b/untitled/Categories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinjalbhattacharyya/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinjalbhattacharyya/IdeaProjects/Google_solutions/untitled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A7A8C0-76C3-7444-B6DB-B868C776F3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D380C1FA-01A6-3248-9907-103CFAC16FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0B0BE18B-0EB5-4F46-A727-E622F804091C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{0B0BE18B-0EB5-4F46-A727-E622F804091C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t>S.no</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Dairy</t>
   </si>
@@ -95,9 +89,6 @@
   </si>
   <si>
     <t>Food Cupboard</t>
-  </si>
-  <si>
-    <t>img url</t>
   </si>
   <si>
     <t>https://www.dairyfoods.com/ext/resources/DF/2020/August/df-100/GettyImages-1194287257.jpg?1597726305</t>
@@ -170,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +173,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -526,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDE005E-6271-4AF1-BCFC-E0074C22FF1E}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -539,198 +536,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>37</v>
@@ -738,59 +735,49 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C21" r:id="rId1" xr:uid="{E4069F9E-8104-40BF-92AE-C6CF78B2F583}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{7E974B6E-1A59-3B42-B89E-9762F3C3CDA3}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{F777771A-BA83-8E44-BE21-2B4C74286ADF}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{FABF6D7C-4D7F-6A44-9CA5-C12C31669813}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{5F654A17-95F1-3945-84BB-944A3CD53854}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{02E13C8E-1790-8547-841C-7E4BB0BCFD39}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{0E0CE62B-D7E3-1F4E-8213-B5B4C8C41050}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{9A7A83DB-CD49-B44A-884B-A8623EEE4FBD}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{8E115AA7-F273-C740-A2EA-2979BA84CBDE}"/>
-    <hyperlink ref="C10" r:id="rId10" xr:uid="{4DC01F09-3B5D-0140-B0DB-9F2044562228}"/>
-    <hyperlink ref="C11" r:id="rId11" location="imgrc=KzWXupJqi7CkVM" xr:uid="{B147ABB2-4E34-B545-B517-307F855BF415}"/>
-    <hyperlink ref="C12" r:id="rId12" xr:uid="{A43343FE-9426-3342-B81D-A74A04C56214}"/>
-    <hyperlink ref="C13" r:id="rId13" xr:uid="{1F1516A0-1FE3-B941-9CA0-A7DE0F4992FA}"/>
-    <hyperlink ref="C14" r:id="rId14" xr:uid="{A5366493-AD2B-BD41-99A7-59B2AC566164}"/>
-    <hyperlink ref="C15" r:id="rId15" xr:uid="{D444F191-7A8E-BB45-B722-D399A5932EC5}"/>
-    <hyperlink ref="C16" r:id="rId16" xr:uid="{0A79923A-48CC-6341-880F-0901C9FAC8AA}"/>
-    <hyperlink ref="C17" r:id="rId17" xr:uid="{DA6A779C-4F34-1A49-977D-B44E830EA454}"/>
-    <hyperlink ref="C18" r:id="rId18" xr:uid="{2ACE2317-DF20-2943-B333-C8C2011A5583}"/>
-    <hyperlink ref="C19" r:id="rId19" xr:uid="{7FAC803E-938B-1042-97DD-8CA014C1790B}"/>
-    <hyperlink ref="C20" r:id="rId20" xr:uid="{4509E305-35C3-9C4E-B225-9A6D4A7C54EF}"/>
+    <hyperlink ref="C20" r:id="rId1" xr:uid="{E4069F9E-8104-40BF-92AE-C6CF78B2F583}"/>
+    <hyperlink ref="C1" r:id="rId2" xr:uid="{7E974B6E-1A59-3B42-B89E-9762F3C3CDA3}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{F777771A-BA83-8E44-BE21-2B4C74286ADF}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{FABF6D7C-4D7F-6A44-9CA5-C12C31669813}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{5F654A17-95F1-3945-84BB-944A3CD53854}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{02E13C8E-1790-8547-841C-7E4BB0BCFD39}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{0E0CE62B-D7E3-1F4E-8213-B5B4C8C41050}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{9A7A83DB-CD49-B44A-884B-A8623EEE4FBD}"/>
+    <hyperlink ref="C8" r:id="rId9" xr:uid="{8E115AA7-F273-C740-A2EA-2979BA84CBDE}"/>
+    <hyperlink ref="C9" r:id="rId10" xr:uid="{4DC01F09-3B5D-0140-B0DB-9F2044562228}"/>
+    <hyperlink ref="C10" r:id="rId11" location="imgrc=KzWXupJqi7CkVM" xr:uid="{B147ABB2-4E34-B545-B517-307F855BF415}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{A43343FE-9426-3342-B81D-A74A04C56214}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{1F1516A0-1FE3-B941-9CA0-A7DE0F4992FA}"/>
+    <hyperlink ref="C13" r:id="rId14" xr:uid="{A5366493-AD2B-BD41-99A7-59B2AC566164}"/>
+    <hyperlink ref="C14" r:id="rId15" xr:uid="{D444F191-7A8E-BB45-B722-D399A5932EC5}"/>
+    <hyperlink ref="C15" r:id="rId16" xr:uid="{0A79923A-48CC-6341-880F-0901C9FAC8AA}"/>
+    <hyperlink ref="C16" r:id="rId17" xr:uid="{DA6A779C-4F34-1A49-977D-B44E830EA454}"/>
+    <hyperlink ref="C17" r:id="rId18" xr:uid="{2ACE2317-DF20-2943-B333-C8C2011A5583}"/>
+    <hyperlink ref="C18" r:id="rId19" xr:uid="{7FAC803E-938B-1042-97DD-8CA014C1790B}"/>
+    <hyperlink ref="C19" r:id="rId20" xr:uid="{4509E305-35C3-9C4E-B225-9A6D4A7C54EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>